<commit_message>
Completed User Creation part Exam Center
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/UsersCreationDetails.xlsx
+++ b/src/test/resources/ExcelFiles/UsersCreationDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12ExamCenter/src/test/resources/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/sahoo_suryakanta_focalpointk12_com/Documents/FP_Automation_Script/ExamCenter_Automation/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{34327670-5C56-469D-83F8-4D5BF2868D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8E93AE0-DACA-4804-B0FE-6C1CB4B5491D}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{34327670-5C56-469D-83F8-4D5BF2868D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{358FA6C5-3F56-4DF5-B7DF-855A2687EBBF}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="2688" windowWidth="20532" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
   <si>
     <t>Email</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Japan1232</t>
+  </si>
+  <si>
+    <t>fpkcontroller</t>
+  </si>
+  <si>
+    <t>159533</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -597,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +675,9 @@
         <v>18</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="G2" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -685,16 +696,18 @@
       <c r="C3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="8">
-        <v>5</v>
+      <c r="D3" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12">
         <v>6644</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -711,11 +724,11 @@
       <c r="C4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="8">
-        <v>5</v>
+      <c r="D4" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F4" s="12">
         <v>9494</v>
@@ -739,11 +752,11 @@
       <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="8">
-        <v>5</v>
+      <c r="D5" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F5" s="12">
         <v>8897</v>
@@ -978,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,7 +1060,9 @@
         <v>18</v>
       </c>
       <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="G2" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
@@ -1077,7 +1092,9 @@
       <c r="F3" s="7">
         <v>6644</v>
       </c>
-      <c r="G3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>

</xml_diff>

<commit_message>
commit location and timeslot creation
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/UsersCreationDetails.xlsx
+++ b/src/test/resources/ExcelFiles/UsersCreationDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/gopi_pagadala_focalpointk12_com/Documents/FPK12 Automation-2024/FPK12ExamCenter/src/test/resources/ExcelFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RavaliManthena\OneDrive\Eclipse-EC\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{34327670-5C56-469D-83F8-4D5BF2868D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8E93AE0-DACA-4804-B0FE-6C1CB4B5491D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11F47F1-D299-4622-B040-D89AC9F9D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5256" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -302,10 +302,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -597,23 +593,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.21875" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="15.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -651,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>21</v>
@@ -675,7 +671,7 @@
       </c>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -701,7 +697,7 @@
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
@@ -729,7 +725,7 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -763,7 +759,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -796,21 +792,21 @@
       <selection activeCell="L2" activeCellId="1" sqref="K2 L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="15.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="20.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.85546875" style="2"/>
     <col min="11" max="11" width="15" style="2" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -848,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="7" t="s">
         <v>23</v>
@@ -872,7 +868,7 @@
       </c>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
@@ -897,7 +893,7 @@
       <c r="J3" s="7"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
@@ -925,7 +921,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
@@ -959,7 +955,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
     </row>
@@ -978,23 +974,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="45.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="18" t="s">
         <v>19</v>
@@ -1058,7 +1054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>32</v>
       </c>
@@ -1082,7 +1078,7 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
@@ -1110,7 +1106,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1144,7 +1140,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="3"/>
     </row>
   </sheetData>

</xml_diff>